<commit_message>
Final updates after conference
</commit_message>
<xml_diff>
--- a/jupyternotebook/reports/multiplicativebadratio.xlsx
+++ b/jupyternotebook/reports/multiplicativebadratio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,97 +438,97 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>ParcelId</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>SaleDate</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SalesPrice</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Sqft</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>LandSize</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bathrooms</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Quality</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>GarageSize</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>EffAge</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>NBHD</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>SPPSF</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>SYEAR</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>SMONTH</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>SDATE</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Months</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Pct_Good</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>ESP</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Ratio</t>
         </is>
@@ -536,123 +536,129 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B2" t="n">
         <v>119180</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="C2" s="2" t="n">
         <v>44939</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>130975</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>1127</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>26275</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>3</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>BelowAverage</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>384</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>11</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>102</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>116.2156166814552</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>2023</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="O2" s="2" t="n">
         <v>44927</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>11</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.89</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>197919</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>1.51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>485</v>
+      </c>
+      <c r="B3" t="n">
         <v>105323</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="C3" s="2" t="n">
         <v>45138</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>76438</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>1200</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>15718</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Poor</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>61</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>101</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>63.69833333333333</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>2023</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>7</v>
       </c>
-      <c r="N3" s="2" t="n">
+      <c r="O3" s="2" t="n">
         <v>45108</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>6</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>5</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.4</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>119194</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>1.56</v>
       </c>
     </row>

</xml_diff>